<commit_message>
New metagenomic dataset, various
Ashish emailed me a new metagenomic dataset that I will perform statistical analysis on to replace the old CAZyme gene domain dataset.

Created a function to generate compact letter displays. The imported function only looks at significantly different pairs, ignoring groups that are "similar" to other groups. The function I created will also create compact letter displays for these other groups.

There are some dependent - independent variable combinations that are missing compact letter displays because Tukey's post-hoc was never performed on them. I will perform Tukey's post-hoc on them and then create compact letter displays using the Tukey's results.
</commit_message>
<xml_diff>
--- a/Statistical analyses/Compact letter displays/Litter chemistry/amide2, interaction, None, Tukey labels.xlsx
+++ b/Statistical analyses/Compact letter displays/Litter chemistry/amide2, interaction, None, Tukey labels.xlsx
@@ -1,40 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LMAOXD\Documents\UCI undergrad\Bio-ESS 199\Microbial-enzyme-activity-in-leaf-litter\Statistical analyses\Compact letter displays\Litter chemistry\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B12A8E-7F0E-40D7-9D41-F27CC04B7078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
-</file>
-
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={BE7B7FAE-60A0-4F32-BB20-4001605A28CC}</author>
-  </authors>
-  <commentList>
-    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{BE7B7FAE-60A0-4F32-BB20-4001605A28CC}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    This row was added manually because the compact letter display module only takes in significant pairs, and this group is not significantly different from any other group</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -46,22 +22,22 @@
     <t>labels</t>
   </si>
   <si>
+    <t>Grassland x Reduced</t>
+  </si>
+  <si>
     <t>CSS x Reduced</t>
   </si>
   <si>
-    <t>Grassland x Reduced</t>
-  </si>
-  <si>
     <t>Grassland x Ambient</t>
   </si>
   <si>
+    <t>CSS x Ambient</t>
+  </si>
+  <si>
     <t>a</t>
   </si>
   <si>
     <t>b</t>
-  </si>
-  <si>
-    <t>CSS x Ambient</t>
   </si>
   <si>
     <t>ab</t>
@@ -70,8 +46,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,12 +62,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -140,27 +110,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Brian Chung" id="{C3ECF399-C951-48C6-9C45-6B21EFD58A39}" userId="fdf24957ba71c53c" providerId="Windows Live"/>
-</personList>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -198,7 +154,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -232,7 +188,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -267,10 +222,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -442,28 +396,15 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="B5" dT="2024-03-11T04:37:59.23" personId="{C3ECF399-C951-48C6-9C45-6B21EFD58A39}" id="{BE7B7FAE-60A0-4F32-BB20-4001605A28CC}">
-    <text>This row was added manually because the compact letter display module only takes in significant pairs, and this group is not significantly different from any other group</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -471,33 +412,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
@@ -505,6 +446,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>